<commit_message>
Alf: add questions regarding some index
</commit_message>
<xml_diff>
--- a/question summary&proper nouns.xlsx
+++ b/question summary&proper nouns.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/libo/work/cargoTrawind/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alf/Desktop/Trawind proj local/TrawindShippingCostForecast/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6819F671-23B4-A048-9815-7A42192A2B1A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C301D682-518F-6744-923A-2B34338EAE10}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="2680" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{7A9FF9E2-8E36-7A49-BD90-F4EB47506221}"/>
+    <workbookView xWindow="4240" yWindow="2680" windowWidth="27640" windowHeight="16940" xr2:uid="{7A9FF9E2-8E36-7A49-BD90-F4EB47506221}"/>
   </bookViews>
   <sheets>
     <sheet name="问题总结" sheetId="2" r:id="rId1"/>
     <sheet name="专有名词" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>公司租船报价</t>
   </si>
@@ -70,6 +70,27 @@
   </si>
   <si>
     <t>预估价格（指导价格）</t>
+  </si>
+  <si>
+    <t>时间</t>
+  </si>
+  <si>
+    <t>提问者</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le </t>
+  </si>
+  <si>
+    <t>我们是否有www.shippingdata.cn （中国航运数据库） 的会员？</t>
+  </si>
+  <si>
+    <t>神海指数中”北“是哪儿？目的地中哪个离镇海比较近？</t>
+  </si>
+  <si>
+    <t>神海指数中2017年和2018年为什么张家港的船型从2 - 3wt 变成了 2-4wt</t>
+  </si>
+  <si>
+    <t>螺纹钢和钢坯价格对运价影响有多大</t>
   </si>
 </sst>
 </file>
@@ -111,10 +132,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -431,54 +458,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6E0B888-6486-EE45-A6AC-B34BB98E147D}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.83203125" customWidth="1"/>
-    <col min="2" max="2" width="128" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="42.83203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="66" style="4" customWidth="1"/>
+    <col min="5" max="5" width="54.1640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:5" ht="126" x14ac:dyDescent="0.2">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" s="4" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="36" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>43444</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>43444</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>43444</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>43444</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -491,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBE94BB-5CFE-0C48-982C-F712A3DC614E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated question list on 12/10/2018
</commit_message>
<xml_diff>
--- a/question summary&proper nouns.xlsx
+++ b/question summary&proper nouns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alf/Desktop/Trawind proj local/TrawindShippingCostForecast/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C301D682-518F-6744-923A-2B34338EAE10}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B5C1DB-912C-1248-8266-37A4C636AC94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4240" yWindow="2680" windowWidth="27640" windowHeight="16940" xr2:uid="{7A9FF9E2-8E36-7A49-BD90-F4EB47506221}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>公司租船报价</t>
   </si>
@@ -90,7 +90,13 @@
     <t>神海指数中2017年和2018年为什么张家港的船型从2 - 3wt 变成了 2-4wt</t>
   </si>
   <si>
-    <t>螺纹钢和钢坯价格对运价影响有多大</t>
+    <t>螺纹钢和钢坯价格对运价影响有多大? 尤其是广州的螺纹钢和钢坯价格</t>
+  </si>
+  <si>
+    <t>动力煤是指的货物为动力煤，还是作为船的燃料？</t>
+  </si>
+  <si>
+    <t>铁矿石的港口库存情况（bloomberg上数据） 是否能对船价产生比较大的影响？</t>
   </si>
 </sst>
 </file>
@@ -458,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6E0B888-6486-EE45-A6AC-B34BB98E147D}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,7 +555,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>43444</v>
       </c>
@@ -558,6 +564,28 @@
       </c>
       <c r="C12" s="4" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>43444</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>43444</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>